<commit_message>
added documentation for model desciption and preliminary results
</commit_message>
<xml_diff>
--- a/rate_matrix_expanded3.xlsx
+++ b/rate_matrix_expanded3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vijetadeshpande/Documents/GitHub/compartmental-model-COVID19/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28DE035-9916-A641-8D60-5E2C144701FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4EA62C-1105-4F4B-8C80-D9AE692172A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{68BC5988-E0E2-3145-9802-2A71AB6DCC1D}"/>
   </bookViews>
@@ -546,7 +546,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -661,8 +661,8 @@
         <v>32</v>
       </c>
       <c r="B4" s="1">
-        <f>(3/10)</f>
-        <v>0.3</v>
+        <f>(3.88/12.5)</f>
+        <v>0.31040000000000001</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -695,8 +695,8 @@
         <v>28</v>
       </c>
       <c r="B5" s="1">
-        <f t="shared" ref="B5:B7" si="0">(3/10)</f>
-        <v>0.3</v>
+        <f t="shared" ref="B5:B8" si="0">(3.88/12.5)</f>
+        <v>0.31040000000000001</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -732,7 +732,7 @@
       </c>
       <c r="B6" s="1">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.31040000000000001</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -768,7 +768,7 @@
       </c>
       <c r="B7" s="1">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.31040000000000001</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>

</xml_diff>